<commit_message>
Add processing species list in ExcelMetadataService
</commit_message>
<xml_diff>
--- a/Src/Hirundo.Databases.Tests.Integration/Assets/example-data.xlsx
+++ b/Src/Hirundo.Databases.Tests.Integration/Assets/example-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Hirundo.NET\Src\Hirundo.Databases.Tests.Integration\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7926D2E9-A6A9-4E2F-9553-140DE7C17B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E507530B-5BDA-4164-9F34-FE283CD97FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="4275" windowWidth="19695" windowHeight="12450" xr2:uid="{42FF3594-03B8-4AE3-976F-2AABAA66A209}"/>
+    <workbookView xWindow="29610" yWindow="2730" windowWidth="19695" windowHeight="12450" xr2:uid="{42FF3594-03B8-4AE3-976F-2AABAA66A209}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>RUB.RUB</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +527,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2">
         <v>24701</v>

</xml_diff>